<commit_message>
nuevo codigo , add colective graphs
</commit_message>
<xml_diff>
--- a/Matches.xlsx
+++ b/Matches.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A776B4-8848-426E-92ED-56C55FB16DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3034C4-5B1C-4FAF-8AED-EC7AC535B585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>fecha</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>visita</t>
+  </si>
+  <si>
+    <t>Tiznados vs USMP</t>
+  </si>
+  <si>
+    <t>USMP</t>
   </si>
 </sst>
 </file>
@@ -147,14 +153,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -438,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +509,7 @@
         <v>46044</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f t="shared" ref="B2" si="0">CONCATENATE(E2,A2)</f>
+        <f t="shared" ref="B2:B3" si="0">CONCATENATE(E2,A2)</f>
         <v>46044</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -530,7 +535,7 @@
         <v>18</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2" si="1">CONCATENATE( "vs ",H2)</f>
+        <f t="shared" ref="L2:L3" si="1">CONCATENATE( "vs ",H2)</f>
         <v>vs Paucarpata X</v>
       </c>
       <c r="M2">
@@ -541,14 +546,50 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="5"/>
-      <c r="H3" s="6"/>
+      <c r="A3" s="2">
+        <v>46064</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>46064</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="str">
+        <f>CONCATENATE(H3,"_",I3)</f>
+        <v>USMP_1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="1"/>
+        <v>vs USMP</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{35DFBE1F-921A-4081-B10D-5E7482E47E31}"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://www.youtube.com/watch?v=vmWdqhzpwTA" xr:uid="{161D1A58-3B6A-4434-B21C-39BF3898F80F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add action type y
</commit_message>
<xml_diff>
--- a/Matches.xlsx
+++ b/Matches.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3034C4-5B1C-4FAF-8AED-EC7AC535B585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D83754-E26F-4CD7-973F-44B46C02D9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,10 +79,10 @@
     <t>visita</t>
   </si>
   <si>
-    <t>Tiznados vs USMP</t>
-  </si>
-  <si>
     <t>USMP</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vmWdqhzpwTA</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +554,7 @@
         <v>46064</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
@@ -563,7 +563,7 @@
         <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -589,7 +589,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{35DFBE1F-921A-4081-B10D-5E7482E47E31}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://www.youtube.com/watch?v=vmWdqhzpwTA" xr:uid="{161D1A58-3B6A-4434-B21C-39BF3898F80F}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{161D1A58-3B6A-4434-B21C-39BF3898F80F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>